<commit_message>
more info on the required APIs
</commit_message>
<xml_diff>
--- a/doc/moodle_api_functions_service_alignment.xlsx
+++ b/doc/moodle_api_functions_service_alignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glah/code/zhaw/moodle-autopilot/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1303D9-1066-BF42-8DBF-A0C776689A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE45D0F-B167-6C4A-AD71-EBE4D1E08996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="500" windowWidth="23620" windowHeight="16160" xr2:uid="{4A1A6958-026D-2A45-AE79-6259C8271175}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3748" uniqueCount="1257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3749" uniqueCount="1257">
   <si>
     <t>Area</t>
   </si>
@@ -4189,8 +4189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E3D07F-206A-2147-86B7-617CA66DDB11}">
   <dimension ref="A1:I591"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C354" workbookViewId="0">
-      <selection activeCell="I369" sqref="I369"/>
+    <sheetView tabSelected="1" topLeftCell="C149" workbookViewId="0">
+      <selection activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7436,7 +7436,7 @@
       </c>
       <c r="G144" s="6"/>
     </row>
-    <row r="145" spans="1:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
         <v>310</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
         <v>310</v>
       </c>
@@ -7483,7 +7483,7 @@
       </c>
       <c r="G146" s="6"/>
     </row>
-    <row r="147" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
         <v>310</v>
       </c>
@@ -7504,7 +7504,7 @@
       </c>
       <c r="G147" s="6"/>
     </row>
-    <row r="148" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
         <v>310</v>
       </c>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="G148" s="6"/>
     </row>
-    <row r="149" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A149" s="6" t="s">
         <v>310</v>
       </c>
@@ -7546,7 +7546,7 @@
       </c>
       <c r="G149" s="6"/>
     </row>
-    <row r="150" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A150" s="6" t="s">
         <v>310</v>
       </c>
@@ -7567,7 +7567,7 @@
       </c>
       <c r="G150" s="6"/>
     </row>
-    <row r="151" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
         <v>310</v>
       </c>
@@ -7588,7 +7588,7 @@
       </c>
       <c r="G151" s="6"/>
     </row>
-    <row r="152" spans="1:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A152" s="6" t="s">
         <v>310</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
         <v>310</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A154" s="6" t="s">
         <v>310</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
         <v>310</v>
       </c>
@@ -7682,7 +7682,7 @@
       <c r="G155" s="6"/>
       <c r="H155" s="6"/>
     </row>
-    <row r="156" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
         <v>310</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
         <v>310</v>
       </c>
@@ -7733,8 +7733,11 @@
       <c r="H157" s="6" t="s">
         <v>1255</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" ht="42" x14ac:dyDescent="0.2">
+      <c r="I157" s="5" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
         <v>310</v>
       </c>
@@ -7758,7 +7761,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A159" s="6" t="s">
         <v>310</v>
       </c>
@@ -7784,7 +7787,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
         <v>310</v>
       </c>

</xml_diff>